<commit_message>
fix vityaz compensator and adjust smg base stats
</commit_message>
<xml_diff>
--- a/changes/9mm-muzzles.xlsx
+++ b/changes/9mm-muzzles.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yifan\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CE49BF86-15C9-4E04-8F27-EF9815771987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0485CB4E-17B0-4CBE-86E3-D95147A3469E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3735" yWindow="4245" windowWidth="28800" windowHeight="15900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="m4-barrels" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>new</t>
   </si>
@@ -216,6 +216,12 @@
   </si>
   <si>
     <t>weight formula</t>
+  </si>
+  <si>
+    <t>izhmash_pp-19-01_vityaz_std_muzzle_brake_compensator</t>
+  </si>
+  <si>
+    <t>Izhmash PP-19-01 Vityaz Std.</t>
   </si>
 </sst>
 </file>
@@ -699,9 +705,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -761,9 +766,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -801,7 +806,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -907,7 +912,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1049,7 +1054,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1057,10 +1062,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q39"/>
+  <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1069,64 +1074,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M2" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N2" t="s">
         <v>3</v>
       </c>
       <c r="P2" t="s">
@@ -1167,7 +1159,7 @@
       <c r="M3">
         <v>100</v>
       </c>
-      <c r="N3" s="1">
+      <c r="N3">
         <f>C3-D3*20-E3*0.8-F3*0.6-H3*5+I3*15+J3/300</f>
         <v>2.8</v>
       </c>
@@ -1203,7 +1195,7 @@
       <c r="M4">
         <v>100</v>
       </c>
-      <c r="N4" s="1">
+      <c r="N4">
         <f t="shared" ref="N4:N25" si="0">C4-D4*20-E4*0.8-F4*0.6-H4*5+I4*15+J4/300</f>
         <v>2.8</v>
       </c>
@@ -1239,7 +1231,7 @@
       <c r="M5">
         <v>500</v>
       </c>
-      <c r="N5" s="1">
+      <c r="N5">
         <f t="shared" si="0"/>
         <v>-1.6166666666666669</v>
       </c>
@@ -1264,7 +1256,7 @@
         <v>-2</v>
       </c>
       <c r="H6">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="I6">
         <v>0</v>
@@ -1275,9 +1267,9 @@
       <c r="M6">
         <v>500</v>
       </c>
-      <c r="N6" s="1">
-        <f t="shared" si="0"/>
-        <v>5.333333333333333</v>
+      <c r="N6">
+        <f t="shared" si="0"/>
+        <v>5.583333333333333</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -1300,7 +1292,7 @@
         <v>-5</v>
       </c>
       <c r="H7">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -1311,9 +1303,9 @@
       <c r="M7">
         <v>600</v>
       </c>
-      <c r="N7" s="1">
-        <f t="shared" si="0"/>
-        <v>7.5666666666666664</v>
+      <c r="N7">
+        <f t="shared" si="0"/>
+        <v>7.8166666666666664</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -1336,40 +1328,40 @@
         <v>-9</v>
       </c>
       <c r="H8">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="I8">
         <v>0</v>
       </c>
       <c r="J8">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="M8">
         <v>1800</v>
       </c>
-      <c r="N8" s="1">
-        <f t="shared" si="0"/>
-        <v>7.666666666666667</v>
+      <c r="N8">
+        <f t="shared" si="0"/>
+        <v>7.8166666666666664</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B9" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D9">
         <v>0.04</v>
       </c>
       <c r="E9">
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="F9">
-        <v>-5</v>
+        <v>-7</v>
       </c>
       <c r="H9">
         <v>0.05</v>
@@ -1378,169 +1370,169 @@
         <v>0</v>
       </c>
       <c r="J9">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="M9">
-        <v>1000</v>
-      </c>
-      <c r="N9" s="1">
-        <f t="shared" si="0"/>
-        <v>6.0166666666666666</v>
+        <v>100</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="0"/>
+        <v>6.9500000000000011</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="C10">
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="D10">
-        <v>0.11</v>
+        <v>0.04</v>
       </c>
       <c r="E10">
         <v>-5</v>
       </c>
       <c r="F10">
-        <v>-7</v>
+        <v>-5</v>
       </c>
       <c r="H10">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="I10">
         <v>0</v>
       </c>
       <c r="J10">
-        <v>-100</v>
+        <v>20</v>
       </c>
       <c r="M10">
         <v>1000</v>
       </c>
-      <c r="N10" s="1">
-        <f t="shared" si="0"/>
-        <v>2.1666666666666665</v>
+      <c r="N10">
+        <f t="shared" si="0"/>
+        <v>6.0166666666666666</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="C11">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="D11">
-        <v>0.18</v>
+        <v>0.11</v>
       </c>
       <c r="E11">
-        <v>-8</v>
+        <v>-5</v>
       </c>
       <c r="F11">
-        <v>-8</v>
+        <v>-7</v>
       </c>
       <c r="H11">
-        <v>-0.05</v>
+        <v>0.1</v>
       </c>
       <c r="I11">
-        <v>7.0000000000000007E-2</v>
+        <v>0</v>
       </c>
       <c r="J11">
-        <v>50</v>
+        <v>-100</v>
       </c>
       <c r="M11">
-        <v>900</v>
-      </c>
-      <c r="N11" s="1">
-        <f t="shared" si="0"/>
-        <v>7.0666666666666673</v>
+        <v>1000</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="0"/>
+        <v>2.1666666666666665</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C12">
-        <v>-4</v>
+        <v>-2</v>
       </c>
       <c r="D12">
-        <v>0.23</v>
+        <v>0.18</v>
       </c>
       <c r="E12">
-        <v>-10</v>
+        <v>-8</v>
       </c>
       <c r="F12">
-        <v>-9</v>
+        <v>-8</v>
       </c>
       <c r="H12">
-        <v>-0.1</v>
+        <v>-0.05</v>
       </c>
       <c r="I12">
-        <v>0.12</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="J12">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="M12">
-        <v>1500</v>
-      </c>
-      <c r="N12" s="1">
-        <f t="shared" si="0"/>
-        <v>7.3666666666666645</v>
+        <v>900</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="0"/>
+        <v>7.0666666666666673</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="C13">
-        <v>-7</v>
+        <v>-4</v>
       </c>
       <c r="D13">
-        <v>0.22</v>
+        <v>0.23</v>
       </c>
       <c r="E13">
-        <v>-7</v>
+        <v>-10</v>
       </c>
       <c r="F13">
-        <v>-8</v>
+        <v>-9</v>
       </c>
       <c r="H13">
-        <v>-0.2</v>
+        <v>-0.1</v>
       </c>
       <c r="I13">
-        <v>0.15</v>
+        <v>0.12</v>
       </c>
       <c r="J13">
-        <v>150</v>
+        <v>80</v>
       </c>
       <c r="M13">
-        <v>1000</v>
-      </c>
-      <c r="N13" s="1">
-        <f t="shared" si="0"/>
-        <v>2.75</v>
+        <v>1500</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="0"/>
+        <v>7.3666666666666645</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C14">
-        <v>-8</v>
+        <v>-7</v>
       </c>
       <c r="D14">
         <v>0.22</v>
@@ -1563,125 +1555,125 @@
       <c r="M14">
         <v>1000</v>
       </c>
-      <c r="N14" s="1">
-        <f t="shared" si="0"/>
-        <v>1.75</v>
+      <c r="N14">
+        <f t="shared" si="0"/>
+        <v>2.75</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C15">
-        <v>-5</v>
+        <v>-8</v>
       </c>
       <c r="D15">
-        <v>0.23</v>
+        <v>0.22</v>
       </c>
       <c r="E15">
-        <v>-10</v>
+        <v>-7</v>
       </c>
       <c r="F15">
-        <v>-10</v>
+        <v>-8</v>
       </c>
       <c r="H15">
         <v>-0.2</v>
       </c>
       <c r="I15">
-        <v>0.13</v>
+        <v>0.15</v>
       </c>
       <c r="J15">
         <v>150</v>
       </c>
       <c r="M15">
-        <v>1200</v>
-      </c>
-      <c r="N15" s="1">
-        <f t="shared" si="0"/>
-        <v>7.8499999999999988</v>
+        <v>1000</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="0"/>
+        <v>1.75</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C16">
         <v>-5</v>
       </c>
       <c r="D16">
-        <v>0.24</v>
+        <v>0.23</v>
       </c>
       <c r="E16">
-        <v>-9</v>
+        <v>-10</v>
       </c>
       <c r="F16">
-        <v>-11</v>
+        <v>-10</v>
       </c>
       <c r="H16">
-        <v>-0.15</v>
+        <v>-0.2</v>
       </c>
       <c r="I16">
-        <v>0.15</v>
+        <v>0.13</v>
       </c>
       <c r="J16">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="M16">
-        <v>1000</v>
-      </c>
-      <c r="N16" s="1">
-        <f t="shared" si="0"/>
-        <v>7.3333333333333321</v>
+        <v>1200</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="0"/>
+        <v>7.8499999999999988</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C17">
-        <v>-6</v>
+        <v>-5</v>
       </c>
       <c r="D17">
-        <v>0.19</v>
+        <v>0.24</v>
       </c>
       <c r="E17">
-        <v>-6</v>
+        <v>-9</v>
       </c>
       <c r="F17">
-        <v>-12</v>
+        <v>-11</v>
       </c>
       <c r="H17">
-        <v>-0.1</v>
+        <v>-0.15</v>
       </c>
       <c r="I17">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="J17">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="M17">
-        <v>1500</v>
-      </c>
-      <c r="N17" s="1">
-        <f t="shared" si="0"/>
-        <v>6.1999999999999993</v>
+        <v>1000</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="0"/>
+        <v>7.3333333333333321</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C18">
         <v>-6</v>
@@ -1707,280 +1699,253 @@
       <c r="M18">
         <v>1500</v>
       </c>
-      <c r="N18" s="1">
+      <c r="N18">
         <f t="shared" si="0"/>
         <v>6.1999999999999993</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="C19">
-        <v>-9</v>
+        <v>-6</v>
       </c>
       <c r="D19">
-        <v>0.25</v>
+        <v>0.19</v>
       </c>
       <c r="E19">
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="F19">
-        <v>-14</v>
+        <v>-12</v>
       </c>
       <c r="H19">
-        <v>-0.2</v>
+        <v>-0.1</v>
       </c>
       <c r="I19">
         <v>0.2</v>
       </c>
       <c r="J19">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="M19">
-        <v>2000</v>
-      </c>
-      <c r="N19" s="1">
-        <f t="shared" si="0"/>
-        <v>3.4000000000000004</v>
+        <v>1500</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="0"/>
+        <v>6.1999999999999993</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20">
+        <v>-9</v>
+      </c>
+      <c r="D20">
+        <v>0.25</v>
+      </c>
+      <c r="E20">
+        <v>-5</v>
+      </c>
+      <c r="F20">
+        <v>-14</v>
+      </c>
+      <c r="H20">
+        <v>-0.2</v>
+      </c>
+      <c r="I20">
+        <v>0.2</v>
+      </c>
+      <c r="J20">
+        <v>300</v>
+      </c>
+      <c r="M20">
+        <v>2000</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="0"/>
+        <v>3.4000000000000004</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>47</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>48</v>
       </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20">
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
         <v>0.03</v>
       </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-      <c r="H20">
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="H21">
         <v>0.05</v>
       </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
-      <c r="J20">
-        <v>0</v>
-      </c>
-      <c r="M20">
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="M21">
         <v>300</v>
       </c>
-      <c r="N20" s="1">
+      <c r="N21">
         <f t="shared" si="0"/>
         <v>-0.85</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>49</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B22" t="s">
         <v>50</v>
       </c>
-      <c r="C21" s="1">
-        <v>0</v>
-      </c>
-      <c r="D21" s="1">
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
         <v>0.03</v>
       </c>
-      <c r="E21" s="1">
-        <v>0</v>
-      </c>
-      <c r="F21" s="1">
-        <v>0</v>
-      </c>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1">
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="H22">
         <v>0.05</v>
       </c>
-      <c r="I21" s="1">
-        <v>0</v>
-      </c>
-      <c r="J21" s="1">
-        <v>0</v>
-      </c>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1">
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="M22">
         <v>300</v>
       </c>
-      <c r="N21" s="1">
+      <c r="N22">
         <f t="shared" si="0"/>
         <v>-0.85</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C23" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D23" s="1">
-        <v>0.09</v>
-      </c>
-      <c r="E23" s="1">
-        <v>-9</v>
-      </c>
-      <c r="F23" s="1">
-        <v>-8</v>
-      </c>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1">
-        <v>-0.1</v>
-      </c>
-      <c r="I23" s="1">
-        <v>0.09</v>
-      </c>
-      <c r="J23" s="1">
-        <v>70</v>
-      </c>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1">
-        <v>1500</v>
-      </c>
-      <c r="N23" s="1">
-        <f t="shared" si="0"/>
-        <v>8.2833333333333332</v>
+      <c r="N23">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B24" t="s">
-        <v>54</v>
-      </c>
-      <c r="C24" s="1">
-        <v>-3</v>
-      </c>
-      <c r="D24" s="1">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="E24" s="1">
-        <v>-3</v>
-      </c>
-      <c r="F24" s="1">
-        <v>-2</v>
+        <v>52</v>
+      </c>
+      <c r="C24">
+        <v>-4</v>
+      </c>
+      <c r="D24">
+        <v>0.09</v>
+      </c>
+      <c r="E24">
+        <v>-9</v>
+      </c>
+      <c r="F24">
+        <v>-8</v>
       </c>
       <c r="H24">
-        <v>-0.05</v>
-      </c>
-      <c r="I24" s="1">
-        <v>0.06</v>
-      </c>
-      <c r="J24" s="1">
-        <v>50</v>
+        <v>-0.1</v>
+      </c>
+      <c r="I24">
+        <v>0.09</v>
+      </c>
+      <c r="J24">
+        <v>70</v>
       </c>
       <c r="M24">
-        <v>1000</v>
-      </c>
-      <c r="N24" s="1">
-        <f t="shared" si="0"/>
-        <v>0.5166666666666665</v>
+        <v>1500</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="0"/>
+        <v>8.2833333333333332</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25">
+        <v>-3</v>
+      </c>
+      <c r="D25">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E25">
+        <v>-3</v>
+      </c>
+      <c r="F25">
+        <v>-2</v>
+      </c>
+      <c r="H25">
+        <v>-0.05</v>
+      </c>
+      <c r="I25">
+        <v>0.06</v>
+      </c>
+      <c r="J25">
+        <v>50</v>
+      </c>
+      <c r="M25">
+        <v>1000</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="0"/>
+        <v>0.5166666666666665</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>55</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>56</v>
       </c>
-      <c r="C25" s="1">
-        <v>0</v>
-      </c>
-      <c r="D25">
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
         <v>0.02</v>
       </c>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="M25">
-        <v>0</v>
-      </c>
-      <c r="N25" s="1">
-        <f t="shared" si="0"/>
+      <c r="M26">
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <f t="shared" ref="N4:N26" si="1">C26-D26*20-E26*0.8-F26*0.6-H26*5+I26*15+J26/300</f>
         <v>-0.4</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="N26" s="1"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="N27" s="1"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="N28" s="1"/>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="N29" s="1"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="N30" s="1"/>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="N31" s="1"/>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="N32" s="1"/>
-    </row>
-    <row r="33" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N33" s="1"/>
-    </row>
-    <row r="34" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N34" s="1"/>
-    </row>
-    <row r="35" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N35" s="1"/>
-    </row>
-    <row r="36" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N36" s="1"/>
-    </row>
-    <row r="37" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N37" s="1"/>
-    </row>
-    <row r="38" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N38" s="1"/>
-    </row>
-    <row r="39" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N39" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>